<commit_message>
bug fixes in noun extraction and telebot.py
</commit_message>
<xml_diff>
--- a/Question_Answers.xlsx
+++ b/Question_Answers.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10513"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8A0FFA34-A261-9A4D-80D5-6D975DE71C72}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6D9E678D-CA1C-0F48-AA2D-0F2703E5D892}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2330,7 +2330,7 @@
   <dimension ref="A1:B632"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B606" workbookViewId="0">
-      <selection activeCell="B617" sqref="B617"/>
+      <selection activeCell="B618" sqref="B618"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>